<commit_message>
upload new design for RCP2Pads
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
+++ b/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Documents\Workspaces\Git\n64rgb\advancedRGBmod\Main-PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Peter\Documents\Workspaces\Git\Mirror\n64rgb\advancedRGBmod\Main-PCB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C52D79F-311E-4527-964A-2CE3D76B68D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
     <sheet name="TOP" sheetId="5" r:id="rId2"/>
     <sheet name="BOT" sheetId="6" r:id="rId3"/>
     <sheet name="THT" sheetId="7" r:id="rId4"/>
+    <sheet name="Flex" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="190">
   <si>
     <t>Designator</t>
   </si>
@@ -619,11 +621,26 @@
       <t>have resistors at the RCP output</t>
     </r>
   </si>
+  <si>
+    <t>Use this if you have resistors at the RCP output, i.e. the flex cable adapter</t>
+  </si>
+  <si>
+    <t>Flex Cable Adapter</t>
+  </si>
+  <si>
+    <t>More information under misc/RCP2Pads/README.md</t>
+  </si>
+  <si>
+    <t>RN1,RN2,RN3,RN4</t>
+  </si>
+  <si>
+    <t>Not marked on silkscreen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1119,21 +1136,16 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1456,51 +1468,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="59.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1526,7 +1536,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1552,7 +1562,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1575,7 +1585,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1601,7 +1611,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1627,7 +1637,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1650,7 +1660,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1673,11 +1683,11 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>52</v>
       </c>
       <c r="C9">
@@ -1702,7 +1712,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1728,7 +1738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -1754,7 +1764,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1780,7 +1790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1806,7 +1816,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1832,7 +1842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1858,7 +1868,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -1884,7 +1894,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1907,7 +1917,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -1927,11 +1937,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>89</v>
       </c>
       <c r="C19">
@@ -1953,7 +1963,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -1979,11 +1989,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>155</v>
       </c>
       <c r="C21">
@@ -1992,7 +2002,7 @@
       <c r="D21" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F21" t="s">
@@ -2008,11 +2018,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>96</v>
       </c>
       <c r="C22">
@@ -2034,7 +2044,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2047,7 +2057,7 @@
       <c r="D23" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F23" t="s">
@@ -2060,7 +2070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -2073,7 +2083,7 @@
       <c r="D24" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F24" t="s">
@@ -2086,7 +2096,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -2099,7 +2109,7 @@
       <c r="D25" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F25" t="s">
@@ -2112,212 +2122,249 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>179</v>
       </c>
-      <c r="C26" s="8">
-        <v>3</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="D27" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F27" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G27" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H27" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I27" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="F27" s="8" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" t="s">
-        <v>181</v>
-      </c>
-      <c r="C28">
+      <c r="G29" t="s">
+        <v>180</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31">
         <v>2</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D31" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" t="s">
+        <v>172</v>
+      </c>
+      <c r="G31" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>188</v>
+      </c>
+      <c r="B34" t="s">
+        <v>179</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
         <v>104</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="E34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>169</v>
-      </c>
-      <c r="B30" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>170</v>
-      </c>
-      <c r="F30" t="s">
-        <v>172</v>
-      </c>
-      <c r="G30" t="s">
-        <v>171</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
+      <c r="G34" t="s">
+        <v>189</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A33:B33"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="I3" r:id="rId4"/>
-    <hyperlink ref="H4" r:id="rId5"/>
-    <hyperlink ref="I10" r:id="rId6"/>
-    <hyperlink ref="H10" r:id="rId7"/>
-    <hyperlink ref="H12" r:id="rId8"/>
-    <hyperlink ref="I12" r:id="rId9"/>
-    <hyperlink ref="H7" r:id="rId10"/>
-    <hyperlink ref="H8" r:id="rId11"/>
-    <hyperlink ref="H9" r:id="rId12"/>
-    <hyperlink ref="H11" r:id="rId13"/>
-    <hyperlink ref="I11" r:id="rId14"/>
-    <hyperlink ref="I13" r:id="rId15"/>
-    <hyperlink ref="H13" r:id="rId16"/>
-    <hyperlink ref="I17" r:id="rId17"/>
-    <hyperlink ref="H14" r:id="rId18"/>
-    <hyperlink ref="I14" r:id="rId19"/>
-    <hyperlink ref="I15" r:id="rId20"/>
-    <hyperlink ref="H15" r:id="rId21"/>
-    <hyperlink ref="H20" r:id="rId22"/>
-    <hyperlink ref="I20" r:id="rId23"/>
-    <hyperlink ref="H19" r:id="rId24"/>
-    <hyperlink ref="I19" r:id="rId25"/>
-    <hyperlink ref="H22" r:id="rId26"/>
-    <hyperlink ref="I22" r:id="rId27"/>
-    <hyperlink ref="I23" r:id="rId28"/>
-    <hyperlink ref="H23" r:id="rId29"/>
-    <hyperlink ref="I24" r:id="rId30"/>
-    <hyperlink ref="H24" r:id="rId31"/>
-    <hyperlink ref="H26" r:id="rId32"/>
-    <hyperlink ref="I26" r:id="rId33"/>
-    <hyperlink ref="I18" r:id="rId34"/>
-    <hyperlink ref="H18" r:id="rId35"/>
-    <hyperlink ref="H21" r:id="rId36"/>
-    <hyperlink ref="I25" r:id="rId37"/>
-    <hyperlink ref="H25" r:id="rId38"/>
-    <hyperlink ref="I28" r:id="rId39"/>
-    <hyperlink ref="H28" r:id="rId40"/>
-    <hyperlink ref="I21" r:id="rId41"/>
-    <hyperlink ref="H6" r:id="rId42"/>
-    <hyperlink ref="H5" r:id="rId43"/>
-    <hyperlink ref="I30" r:id="rId44"/>
-    <hyperlink ref="H30" r:id="rId45"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="I11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I13" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H13" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="I17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="I15" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H20" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="I20" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H19" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="I19" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H22" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="I22" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="I23" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H23" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="I24" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H24" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H27" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="I27" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="I18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H18" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H21" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="I25" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H25" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="I29" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H29" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="I21" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="H6" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="H5" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="I31" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="H31" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="H34" r:id="rId46" xr:uid="{5E57E63F-33D6-428A-ABCB-5B8567D57C33}"/>
+    <hyperlink ref="I34" r:id="rId47" xr:uid="{08919C78-A01D-4C57-B82C-59DAF2016E99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId48"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H20:I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="59.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2339,7 +2386,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2361,7 +2408,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2380,7 +2427,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2402,7 +2449,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2421,7 +2468,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2440,11 +2487,11 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>52</v>
       </c>
       <c r="C8">
@@ -2465,7 +2512,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -2487,7 +2534,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -2509,7 +2556,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>146</v>
       </c>
@@ -2531,7 +2578,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2553,7 +2600,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2575,7 +2622,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -2597,7 +2644,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -2616,7 +2663,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -2638,11 +2685,11 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>155</v>
       </c>
       <c r="C17">
@@ -2651,7 +2698,7 @@
       <c r="D17" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>151</v>
       </c>
       <c r="F17" t="s">
@@ -2663,11 +2710,11 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>96</v>
       </c>
       <c r="C18">
@@ -2685,7 +2732,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2698,7 +2745,7 @@
       <c r="D19" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F19" t="s">
@@ -2707,7 +2754,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -2720,7 +2767,7 @@
       <c r="D20" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F20" t="s">
@@ -2729,51 +2776,51 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" t="s">
         <v>176</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -2786,22 +2833,22 @@
       <c r="D23" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F23" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" t="s">
         <v>180</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
   </sheetData>
@@ -2810,45 +2857,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="59.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2870,7 +2917,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -2892,7 +2939,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>144</v>
       </c>
@@ -2914,7 +2961,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -2936,11 +2983,11 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>89</v>
       </c>
       <c r="C6">
@@ -2958,7 +3005,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -2980,11 +3027,11 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>96</v>
       </c>
       <c r="C8">
@@ -3002,7 +3049,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -3015,7 +3062,7 @@
       <c r="D9" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F9" t="s">
@@ -3024,7 +3071,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -3044,10 +3091,10 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
     </row>
   </sheetData>
@@ -3056,43 +3103,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="59.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -3108,60 +3155,184 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="E5" s="3"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="3"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="3"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="3"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B6EFBF-BD11-4B9B-951C-58BA953094E0}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="59.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E12" s="2"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bank separation between digital video in and digital video outs using 2.5V LDO
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
+++ b/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Peter\Documents\Workspaces\Git\Mirror\n64rgb\advancedRGBmod\Main-PCB\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Workspaces\Git\CoSA-GitLab\n64rgb\advancedRGBmod\Main-PCB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C52D79F-311E-4527-964A-2CE3D76B68D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
@@ -181,15 +180,9 @@
     <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70012DDCR/296-39275-1-ND/</t>
   </si>
   <si>
-    <t>TLV70025DDCR</t>
-  </si>
-  <si>
     <t>LDO 2.5V</t>
   </si>
   <si>
-    <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70025DDCR/296-32411-1-ND/</t>
-  </si>
-  <si>
     <t xml:space="preserve">ASE-50.000MHZ-LC-T </t>
   </si>
   <si>
@@ -530,9 +523,6 @@
   </si>
   <si>
     <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70012DDCR?qs=sGAEpiMZZMsGz1a6aV8DcFnW8%252bX0rdBC2IduztBAJN4%3d</t>
-  </si>
-  <si>
-    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70025DDCR?qs=sGAEpiMZZMsGz1a6aV8DcCniYaGUA430fOrmgOH3ksU%3d</t>
   </si>
   <si>
     <t>https://www.mouser.de/ProductDetail/ABRACON/ASE-50000MHZ-L-C-T?qs=%2fha2pyFaduiJXabh5egm1N76js19RDbbd6bevDP%252bnxvNwEFIULtJfwJQd%2f%252bio1%252bk</t>
@@ -636,11 +626,20 @@
   <si>
     <t>Not marked on silkscreen</t>
   </si>
+  <si>
+    <t>TLV70225DBVR</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70225DBVR?qs=sGAEpiMZZMsGz1a6aV8DcOCbyvSkQ88lxvyfqcpx5P4%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70225DBVR/296-37705-1-ND/4833933</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1468,20 +1467,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="59.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1510,18 +1509,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -1530,18 +1529,18 @@
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1553,16 +1552,16 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1582,62 +1581,62 @@
         <v>36</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
         <v>44</v>
       </c>
       <c r="G6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1657,64 +1656,64 @@
         <v>48</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>49</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
       </c>
       <c r="F8" t="s">
         <v>47</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>51</v>
+        <v>189</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
       <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>53</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>56</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -1726,7 +1725,7 @@
         <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>
@@ -1738,9 +1737,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1749,27 +1748,27 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -1778,7 +1777,7 @@
         <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
@@ -1790,9 +1789,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -1801,22 +1800,22 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F13" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1830,19 +1829,19 @@
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1856,24 +1855,24 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
         <v>30</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1882,169 +1881,169 @@
         <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F17" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" t="s">
         <v>109</v>
       </c>
-      <c r="B18" t="s">
-        <v>111</v>
-      </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" t="s">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
         <v>85</v>
-      </c>
-      <c r="F19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" t="s">
-        <v>87</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" t="s">
         <v>151</v>
       </c>
-      <c r="F21" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" t="s">
-        <v>153</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F22" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2055,216 +2054,216 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
         <v>97</v>
       </c>
-      <c r="F23" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="1" t="s">
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F24" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="I25" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F26" t="s">
         <v>30</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F27" t="s">
         <v>30</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
         <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" t="s">
+        <v>167</v>
+      </c>
+      <c r="F31" t="s">
+        <v>169</v>
+      </c>
+      <c r="G31" t="s">
+        <v>168</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F31" t="s">
-        <v>172</v>
-      </c>
-      <c r="G31" t="s">
-        <v>171</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" t="s">
         <v>30</v>
       </c>
       <c r="G34" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2272,76 +2271,73 @@
     <mergeCell ref="A33:B33"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="I10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="I12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="H7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="H8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="H9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="H11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="I11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="I13" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="H13" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="I17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="H14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="I14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="I15" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="H15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="H20" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="I20" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="H19" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="I19" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="H22" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="I22" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="I23" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="H23" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="I24" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="H24" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="H27" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="I27" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="I18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="H18" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="H21" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="I25" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H25" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="I29" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="H29" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="I21" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="H6" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="H5" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="I31" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="H31" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="H34" r:id="rId46" xr:uid="{5E57E63F-33D6-428A-ABCB-5B8567D57C33}"/>
-    <hyperlink ref="I34" r:id="rId47" xr:uid="{08919C78-A01D-4C57-B82C-59DAF2016E99}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="I3" r:id="rId4"/>
+    <hyperlink ref="H4" r:id="rId5"/>
+    <hyperlink ref="I10" r:id="rId6"/>
+    <hyperlink ref="H10" r:id="rId7"/>
+    <hyperlink ref="H12" r:id="rId8"/>
+    <hyperlink ref="I12" r:id="rId9"/>
+    <hyperlink ref="H7" r:id="rId10"/>
+    <hyperlink ref="H9" r:id="rId11"/>
+    <hyperlink ref="H11" r:id="rId12"/>
+    <hyperlink ref="I11" r:id="rId13"/>
+    <hyperlink ref="I13" r:id="rId14"/>
+    <hyperlink ref="H13" r:id="rId15"/>
+    <hyperlink ref="I17" r:id="rId16"/>
+    <hyperlink ref="H14" r:id="rId17"/>
+    <hyperlink ref="I14" r:id="rId18"/>
+    <hyperlink ref="I15" r:id="rId19"/>
+    <hyperlink ref="H15" r:id="rId20"/>
+    <hyperlink ref="H20" r:id="rId21"/>
+    <hyperlink ref="I20" r:id="rId22"/>
+    <hyperlink ref="H19" r:id="rId23"/>
+    <hyperlink ref="I19" r:id="rId24"/>
+    <hyperlink ref="H22" r:id="rId25"/>
+    <hyperlink ref="I22" r:id="rId26"/>
+    <hyperlink ref="I23" r:id="rId27"/>
+    <hyperlink ref="H23" r:id="rId28"/>
+    <hyperlink ref="I24" r:id="rId29"/>
+    <hyperlink ref="H24" r:id="rId30"/>
+    <hyperlink ref="H27" r:id="rId31"/>
+    <hyperlink ref="I27" r:id="rId32"/>
+    <hyperlink ref="I18" r:id="rId33"/>
+    <hyperlink ref="H18" r:id="rId34"/>
+    <hyperlink ref="H21" r:id="rId35"/>
+    <hyperlink ref="I25" r:id="rId36"/>
+    <hyperlink ref="H25" r:id="rId37"/>
+    <hyperlink ref="I29" r:id="rId38"/>
+    <hyperlink ref="H29" r:id="rId39"/>
+    <hyperlink ref="I21" r:id="rId40"/>
+    <hyperlink ref="H6" r:id="rId41"/>
+    <hyperlink ref="H5" r:id="rId42"/>
+    <hyperlink ref="I31" r:id="rId43"/>
+    <hyperlink ref="H31" r:id="rId44"/>
+    <hyperlink ref="H34" r:id="rId45"/>
+    <hyperlink ref="I34" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId48"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H20:I24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="59.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2364,18 +2360,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -2386,12 +2382,12 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2403,12 +2399,12 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2427,29 +2423,29 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2468,18 +2464,18 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
       <c r="B7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>49</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
       </c>
       <c r="F7" t="s">
         <v>47</v>
@@ -2487,34 +2483,34 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
       <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -2526,7 +2522,7 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
         <v>31</v>
@@ -2534,12 +2530,12 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2548,7 +2544,7 @@
         <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>
@@ -2556,9 +2552,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -2567,18 +2563,18 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2592,15 +2588,15 @@
         <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2614,7 +2610,7 @@
         <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
         <v>30</v>
@@ -2622,12 +2618,12 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -2636,103 +2632,103 @@
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
         <v>151</v>
-      </c>
-      <c r="F17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" t="s">
-        <v>153</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2743,112 +2739,112 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F21" t="s">
         <v>30</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F22" t="s">
         <v>30</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F23" t="s">
         <v>30</v>
       </c>
       <c r="G23" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
   </sheetData>
@@ -2857,22 +2853,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="59.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2895,31 +2891,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>127</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>129</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -2928,23 +2924,23 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2953,7 +2949,7 @@
         <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
@@ -2961,9 +2957,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2972,129 +2968,129 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
         <v>83</v>
       </c>
-      <c r="E6" t="s">
-        <v>85</v>
-      </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
   </sheetData>
@@ -3103,20 +3099,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="59.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3139,68 +3135,68 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
         <v>109</v>
       </c>
-      <c r="B2" t="s">
-        <v>111</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="2"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="2"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
   </sheetData>
@@ -3209,31 +3205,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B6EFBF-BD11-4B9B-951C-58BA953094E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="59.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -3256,77 +3252,77 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="2"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="2"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" s="2"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update N64Adv board: - csync level selection by jumper - output IO bank powered by 5V rail (over a 3.3V ldo)
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
+++ b/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Workspaces\Git\CoSA-GitLab\n64rgb\advancedRGBmod\Main-PCB\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\Git\Eigenes\n64rgb\advancedRGBmod\Main-PCB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4301A9D6-E270-49B7-B8FB-2B6C0CA40989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
+    <workbookView xWindow="1035" yWindow="3390" windowWidth="23955" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
     <sheet name="TOP" sheetId="5" r:id="rId2"/>
     <sheet name="BOT" sheetId="6" r:id="rId3"/>
     <sheet name="THT" sheetId="7" r:id="rId4"/>
-    <sheet name="Flex" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="181029" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="184">
   <si>
     <t>Designator</t>
   </si>
@@ -57,12 +63,6 @@
     <t>TSH122ICT</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM31CR60J226KE19L </t>
-  </si>
-  <si>
-    <t>GRM32DR60J336ME19L</t>
-  </si>
-  <si>
     <t>GRM188R70J103KA01D</t>
   </si>
   <si>
@@ -72,9 +72,6 @@
     <t>R11</t>
   </si>
   <si>
-    <t>RC0603FR-07475RL</t>
-  </si>
-  <si>
     <t>MPN</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>EQFP144</t>
   </si>
   <si>
-    <t>can be replaced with other FPGAs on demand (see Schematic file)</t>
-  </si>
-  <si>
     <t>Video DAC 8bit, 3Ch.</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>SMD0805</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Murata-Electronics/GRM32DR60J336ME19L/</t>
-  </si>
-  <si>
     <t>GRM219R60J476ME44D</t>
   </si>
   <si>
@@ -204,9 +195,6 @@
     <t>C1,C2</t>
   </si>
   <si>
-    <t>C101,C121,C301</t>
-  </si>
-  <si>
     <t>Ceramic capacitor, X7R</t>
   </si>
   <si>
@@ -240,9 +228,6 @@
     <t>C202,C204,C206,C302,C801</t>
   </si>
   <si>
-    <t>FB1,FB2,FB3,FB4</t>
-  </si>
-  <si>
     <t>MPZ1608S221A</t>
   </si>
   <si>
@@ -258,21 +243,9 @@
     <t>C21,C22,C102,C103,C104,C105,C106,C107,C108,C109,C110,C111,C112,C113,C122,C123,C124,C125,C126,C127,C128,C129,C131,C132,C141,C142,C201,C203,C205,C401,C501</t>
   </si>
   <si>
-    <t>SMD1210</t>
-  </si>
-  <si>
     <t>33uF / 6.3V</t>
   </si>
   <si>
-    <t>https://www.digikey.de/product-detail/de/murata-electronics-north-america/GRM32DR60J336ME19L/490-3389-1-ND/</t>
-  </si>
-  <si>
-    <t>http://www.mouser.de/ProductDetail/Murata/GRM31CR60J226KE19L/</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/product-detail/de/murata-electronics-north-america/GRM31CR60J226KE19L/</t>
-  </si>
-  <si>
     <t>22uF / 6.3V</t>
   </si>
   <si>
@@ -303,9 +276,6 @@
     <t>http://www.mouser.de/ProductDetail/Yageo/RC0603FR-071KL/</t>
   </si>
   <si>
-    <t>R21</t>
-  </si>
-  <si>
     <t>4k7</t>
   </si>
   <si>
@@ -318,21 +288,12 @@
     <t xml:space="preserve">RC0603FR-074K7L </t>
   </si>
   <si>
-    <t>475</t>
-  </si>
-  <si>
     <t>75</t>
   </si>
   <si>
     <t>RC0603FR-0775RL</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Yageo/RC0603FR-07475RL/</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/product-detail/de/yageo/RC0603FR-07475RL/311-475HRCT-ND/</t>
-  </si>
-  <si>
     <t>http://www.mouser.de/ProductDetail/Yageo/RC0603FR-0775RL/</t>
   </si>
   <si>
@@ -378,9 +339,6 @@
     <t>GRM21BR60J106ME19L</t>
   </si>
   <si>
-    <t>R33</t>
-  </si>
-  <si>
     <t>http://www.mouser.de/search/ProductDetail.aspx?R=0virtualkey0virtualkeyCAT16-75R0F4LF</t>
   </si>
   <si>
@@ -441,9 +399,6 @@
     <t>Non-Inv Buffer 3Ch., Schmitt Trigger</t>
   </si>
   <si>
-    <t>C601,C602,C701,C702</t>
-  </si>
-  <si>
     <t>GRM18R60J105KA01J</t>
   </si>
   <si>
@@ -456,9 +411,6 @@
     <t>1uF / 6.3V</t>
   </si>
   <si>
-    <t>C121,C301</t>
-  </si>
-  <si>
     <t>C101</t>
   </si>
   <si>
@@ -480,13 +432,7 @@
     <t>R22,R52,R53</t>
   </si>
   <si>
-    <t>518</t>
-  </si>
-  <si>
     <t>http://www.mouser.de/ProductDetail/Yageo/RC0603FR-07523RL/</t>
-  </si>
-  <si>
-    <t>with ADV7123: use 516ohm resistor; for PAL-Standard: 528ohm/527ohm</t>
   </si>
   <si>
     <t>https://www.digikey.de/product-detail/de/yageo/RC0603FR-07523RL/311-523HRCT-ND/</t>
@@ -615,31 +561,73 @@
     <t>Use this if you have resistors at the RCP output, i.e. the flex cable adapter</t>
   </si>
   <si>
-    <t>Flex Cable Adapter</t>
-  </si>
-  <si>
-    <t>More information under misc/RCP2Pads/README.md</t>
-  </si>
-  <si>
-    <t>RN1,RN2,RN3,RN4</t>
-  </si>
-  <si>
-    <t>Not marked on silkscreen</t>
-  </si>
-  <si>
-    <t>TLV70225DBVR</t>
-  </si>
-  <si>
     <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70225DBVR?qs=sGAEpiMZZMsGz1a6aV8DcOCbyvSkQ88lxvyfqcpx5P4%3D</t>
   </si>
   <si>
     <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70225DBVR/296-37705-1-ND/4833933</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>TLV70025DDCR</t>
+  </si>
+  <si>
+    <t>TLV70033DDCR</t>
+  </si>
+  <si>
+    <t>LDO 3.3V</t>
+  </si>
+  <si>
+    <t>C101,C114,C121,C301</t>
+  </si>
+  <si>
+    <t>C601,C602,C701,C702,C901,C902</t>
+  </si>
+  <si>
+    <t>QTY/PCB</t>
+  </si>
+  <si>
+    <t>Number of PCBs</t>
+  </si>
+  <si>
+    <t>FB1,FB2,FB3,FB4,FB5</t>
+  </si>
+  <si>
+    <t>C116,C121,C301</t>
+  </si>
+  <si>
+    <t>Cyclone IV FPGA, 10k LE</t>
+  </si>
+  <si>
+    <t>EP4CE10E22C8N</t>
+  </si>
+  <si>
+    <t>Alternative to Cyclone 10 LP FPGA</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R21,R33</t>
+  </si>
+  <si>
+    <t>R21 with ADV7123: use 516ohm resistor; for PAL-Standard: 528ohm/527ohm</t>
+  </si>
+  <si>
+    <t>6k19</t>
+  </si>
+  <si>
+    <t>RC0603FR-076K19L</t>
+  </si>
+  <si>
+    <t>523</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1144,7 +1132,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1467,865 +1455,959 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f>$C$1*C4</f>
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D35" si="0">$C$1*C6</f>
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D14">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="I14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>155</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>31</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="E15" t="s">
         <v>52</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F15" t="s">
         <v>53</v>
       </c>
-      <c r="G9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G15" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="I15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
-        <v>38</v>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
         <v>69</v>
       </c>
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>110</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21">
         <v>5</v>
       </c>
-      <c r="D20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21" t="s">
-        <v>62</v>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
       </c>
       <c r="G21" t="s">
-        <v>151</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>152</v>
+        <v>56</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
       </c>
       <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G25" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" t="s">
+        <v>180</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E22" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>178</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F22" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="G29" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="J29" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="1" t="s">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>153</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I24" s="1" t="s">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" t="s">
+        <v>157</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26" t="s">
-        <v>173</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35">
         <v>2</v>
       </c>
-      <c r="D29" t="s">
-        <v>102</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" t="s">
-        <v>177</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>166</v>
-      </c>
-      <c r="B31" t="s">
-        <v>165</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" t="s">
-        <v>169</v>
-      </c>
-      <c r="G31" t="s">
-        <v>168</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>185</v>
-      </c>
-      <c r="B34" t="s">
-        <v>176</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F34" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" t="s">
-        <v>186</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>117</v>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" t="s">
+        <v>149</v>
+      </c>
+      <c r="H35" t="s">
+        <v>148</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="I3" r:id="rId4"/>
-    <hyperlink ref="H4" r:id="rId5"/>
-    <hyperlink ref="I10" r:id="rId6"/>
-    <hyperlink ref="H10" r:id="rId7"/>
-    <hyperlink ref="H12" r:id="rId8"/>
-    <hyperlink ref="I12" r:id="rId9"/>
-    <hyperlink ref="H7" r:id="rId10"/>
-    <hyperlink ref="H9" r:id="rId11"/>
-    <hyperlink ref="H11" r:id="rId12"/>
-    <hyperlink ref="I11" r:id="rId13"/>
-    <hyperlink ref="I13" r:id="rId14"/>
-    <hyperlink ref="H13" r:id="rId15"/>
-    <hyperlink ref="I17" r:id="rId16"/>
-    <hyperlink ref="H14" r:id="rId17"/>
-    <hyperlink ref="I14" r:id="rId18"/>
-    <hyperlink ref="I15" r:id="rId19"/>
-    <hyperlink ref="H15" r:id="rId20"/>
-    <hyperlink ref="H20" r:id="rId21"/>
-    <hyperlink ref="I20" r:id="rId22"/>
-    <hyperlink ref="H19" r:id="rId23"/>
-    <hyperlink ref="I19" r:id="rId24"/>
-    <hyperlink ref="H22" r:id="rId25"/>
-    <hyperlink ref="I22" r:id="rId26"/>
-    <hyperlink ref="I23" r:id="rId27"/>
-    <hyperlink ref="H23" r:id="rId28"/>
-    <hyperlink ref="I24" r:id="rId29"/>
-    <hyperlink ref="H24" r:id="rId30"/>
-    <hyperlink ref="H27" r:id="rId31"/>
-    <hyperlink ref="I27" r:id="rId32"/>
-    <hyperlink ref="I18" r:id="rId33"/>
-    <hyperlink ref="H18" r:id="rId34"/>
-    <hyperlink ref="H21" r:id="rId35"/>
-    <hyperlink ref="I25" r:id="rId36"/>
-    <hyperlink ref="H25" r:id="rId37"/>
-    <hyperlink ref="I29" r:id="rId38"/>
-    <hyperlink ref="H29" r:id="rId39"/>
-    <hyperlink ref="I21" r:id="rId40"/>
-    <hyperlink ref="H6" r:id="rId41"/>
-    <hyperlink ref="H5" r:id="rId42"/>
-    <hyperlink ref="I31" r:id="rId43"/>
-    <hyperlink ref="H31" r:id="rId44"/>
-    <hyperlink ref="H34" r:id="rId45"/>
-    <hyperlink ref="I34" r:id="rId46"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="I15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="J17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="J21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="I24" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="I26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="J28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="I28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="I31" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="J31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="J22" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="I22" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="I25" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="J29" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="I29" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="J33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="I33" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="J25" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="I9" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="I8" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="J35" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="I35" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2342,22 +2424,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2365,19 +2447,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2387,19 +2466,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2415,437 +2494,450 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
-      </c>
-      <c r="B14" t="s">
-        <v>137</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>123</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>149</v>
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s">
-        <v>91</v>
+        <v>70</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="G18" t="s">
+        <v>180</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>95</v>
+        <v>70</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>96</v>
+        <v>181</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>181</v>
+        <v>56</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>172</v>
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>87</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>123</v>
-      </c>
-      <c r="B23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
+      <c r="B23" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" t="s">
-        <v>177</v>
+        <v>26</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2853,7 +2945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2873,218 +2965,218 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="G11" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3099,7 +3191,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3117,36 +3209,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3202,133 +3294,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>186</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="2"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="2"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update BOM for new flex cable concept
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
+++ b/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\Git\Eigenes\n64rgb\advancedRGBmod\Main-PCB\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Peter\Documents\Workspaces\GitHub\n64rgb\advancedRGBmod\Main-PCB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4301A9D6-E270-49B7-B8FB-2B6C0CA40989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD8E436-2E03-4837-BF18-63A12544EB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="3390" windowWidth="23955" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="183">
   <si>
     <t>Designator</t>
   </si>
@@ -504,9 +504,6 @@
     <t>BD 120OHMS 25%</t>
   </si>
   <si>
-    <t>Use this if you have resistors at the RCP output</t>
-  </si>
-  <si>
     <t>CAT16-47R0F4LF / CAY16-47R0F4LF</t>
   </si>
   <si>
@@ -522,16 +519,74 @@
     <t>https://www.digikey.de/product-detail/de/taiyo-yuden/BK32164M121-T/587-2689-1-ND/2417276</t>
   </si>
   <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70225DBVR?qs=sGAEpiMZZMsGz1a6aV8DcOCbyvSkQ88lxvyfqcpx5P4%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70225DBVR/296-37705-1-ND/4833933</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>TLV70025DDCR</t>
+  </si>
+  <si>
+    <t>TLV70033DDCR</t>
+  </si>
+  <si>
+    <t>LDO 3.3V</t>
+  </si>
+  <si>
+    <t>C101,C114,C121,C301</t>
+  </si>
+  <si>
+    <t>C601,C602,C701,C702,C901,C902</t>
+  </si>
+  <si>
+    <t>QTY/PCB</t>
+  </si>
+  <si>
+    <t>Number of PCBs</t>
+  </si>
+  <si>
+    <t>FB1,FB2,FB3,FB4,FB5</t>
+  </si>
+  <si>
+    <t>C116,C121,C301</t>
+  </si>
+  <si>
+    <t>Cyclone IV FPGA, 10k LE</t>
+  </si>
+  <si>
+    <t>EP4CE10E22C8N</t>
+  </si>
+  <si>
+    <t>Alternative to Cyclone 10 LP FPGA</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R21,R33</t>
+  </si>
+  <si>
+    <t>R21 with ADV7123: use 516ohm resistor; for PAL-Standard: 528ohm/527ohm</t>
+  </si>
+  <si>
+    <t>6k19</t>
+  </si>
+  <si>
+    <t>RC0603FR-076K19L</t>
+  </si>
+  <si>
+    <t>523</t>
+  </si>
+  <si>
+    <t>Use this alternative if you have resistors at the RCP output, e.g. with the "old" flex cable adapter</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Only use this if you </t>
+      <t xml:space="preserve">Use this if you </t>
     </r>
     <r>
       <rPr>
@@ -554,74 +609,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>have resistors at the RCP output</t>
+      <t>have resistors at the RCP output or if you use a flex with buffer Ics</t>
     </r>
-  </si>
-  <si>
-    <t>Use this if you have resistors at the RCP output, i.e. the flex cable adapter</t>
-  </si>
-  <si>
-    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70225DBVR?qs=sGAEpiMZZMsGz1a6aV8DcOCbyvSkQ88lxvyfqcpx5P4%3D</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70225DBVR/296-37705-1-ND/4833933</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>TLV70025DDCR</t>
-  </si>
-  <si>
-    <t>TLV70033DDCR</t>
-  </si>
-  <si>
-    <t>LDO 3.3V</t>
-  </si>
-  <si>
-    <t>C101,C114,C121,C301</t>
-  </si>
-  <si>
-    <t>C601,C602,C701,C702,C901,C902</t>
-  </si>
-  <si>
-    <t>QTY/PCB</t>
-  </si>
-  <si>
-    <t>Number of PCBs</t>
-  </si>
-  <si>
-    <t>FB1,FB2,FB3,FB4,FB5</t>
-  </si>
-  <si>
-    <t>C116,C121,C301</t>
-  </si>
-  <si>
-    <t>Cyclone IV FPGA, 10k LE</t>
-  </si>
-  <si>
-    <t>EP4CE10E22C8N</t>
-  </si>
-  <si>
-    <t>Alternative to Cyclone 10 LP FPGA</t>
-  </si>
-  <si>
-    <t>R34</t>
-  </si>
-  <si>
-    <t>R21,R33</t>
-  </si>
-  <si>
-    <t>R21 with ADV7123: use 516ohm resistor; for PAL-Standard: 528ohm/527ohm</t>
-  </si>
-  <si>
-    <t>6k19</t>
-  </si>
-  <si>
-    <t>RC0603FR-076K19L</t>
-  </si>
-  <si>
-    <t>523</t>
   </si>
 </sst>
 </file>
@@ -1472,7 +1461,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1">
@@ -1487,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>12</v>
@@ -1540,16 +1529,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1703,7 +1692,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1719,10 +1708,10 @@
         <v>42</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1760,10 +1749,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1773,7 +1762,7 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G13" t="s">
         <v>42</v>
@@ -1843,7 +1832,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
         <v>99</v>
@@ -1949,7 +1938,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
         <v>120</v>
@@ -1979,7 +1968,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
         <v>63</v>
@@ -2090,7 +2079,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
         <v>133</v>
@@ -2106,13 +2095,13 @@
         <v>70</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G25" t="s">
         <v>56</v>
       </c>
       <c r="H25" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>132</v>
@@ -2156,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2169,7 +2158,7 @@
         <v>70</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G27" t="s">
         <v>56</v>
@@ -2179,7 +2168,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s">
         <v>84</v>
@@ -2241,56 +2230,56 @@
       <c r="A30" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>152</v>
+      <c r="B30" t="s">
+        <v>155</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f>$C$1*C30</f>
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
       <c r="G30" t="s">
         <v>26</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>156</v>
+      <c r="B31" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="G31" t="s">
         <v>26</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2298,7 +2287,7 @@
         <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -2317,7 +2306,7 @@
         <v>26</v>
       </c>
       <c r="H33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>103</v>
@@ -2385,8 +2374,8 @@
     <hyperlink ref="J26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="J28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="I28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="I31" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="J31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="I30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="J30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="J22" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="I22" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="I25" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
@@ -2409,7 +2398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2548,7 +2539,7 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2589,16 +2580,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>165</v>
-      </c>
-      <c r="B9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>168</v>
       </c>
       <c r="F9" t="s">
         <v>42</v>
@@ -2630,7 +2621,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -2712,7 +2703,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
         <v>120</v>
@@ -2734,7 +2725,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B16" t="s">
         <v>63</v>
@@ -2775,7 +2766,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B18" t="s">
         <v>133</v>
@@ -2787,13 +2778,13 @@
         <v>70</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F18" t="s">
         <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2825,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2834,7 +2825,7 @@
         <v>70</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F20" t="s">
         <v>56</v>
@@ -2844,7 +2835,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
@@ -2869,7 +2860,7 @@
         <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -2884,9 +2875,8 @@
         <v>26</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H22" s="1"/>
+        <v>182</v>
+      </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2903,9 +2893,8 @@
         <v>26</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H23" s="1"/>
+        <v>181</v>
+      </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2913,7 +2902,7 @@
         <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -2928,7 +2917,7 @@
         <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>

</xml_diff>

<commit_message>
bugfix: repair url to correct IC @ U7
</commit_message>
<xml_diff>
--- a/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
+++ b/advancedRGBmod/Main-PCB/doc/n64adv_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Peter\Documents\Workspaces\GitHub\n64rgb\advancedRGBmod\Main-PCB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD8E436-2E03-4837-BF18-63A12544EB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99A7243-AE14-4910-B636-E91D776FCF93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3765" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_N64_Advanced" sheetId="1" r:id="rId1"/>
@@ -519,12 +519,6 @@
     <t>https://www.digikey.de/product-detail/de/taiyo-yuden/BK32164M121-T/587-2689-1-ND/2417276</t>
   </si>
   <si>
-    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70225DBVR?qs=sGAEpiMZZMsGz1a6aV8DcOCbyvSkQ88lxvyfqcpx5P4%3D</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70225DBVR/296-37705-1-ND/4833933</t>
-  </si>
-  <si>
     <t>U9</t>
   </si>
   <si>
@@ -611,6 +605,12 @@
       </rPr>
       <t>have resistors at the RCP output or if you use a flex with buffer Ics</t>
     </r>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/TLV70025DDCR?qs=DS7Z8uEdLNxV6KqAL09ERw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/product-detail/de/texas-instruments/TLV70025DDCR/296-32411-1-ND/3505569</t>
   </si>
 </sst>
 </file>
@@ -1461,7 +1461,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1">
@@ -1476,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>12</v>
@@ -1529,16 +1529,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1692,7 +1692,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1708,10 +1708,10 @@
         <v>42</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1749,10 +1749,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" t="s">
         <v>162</v>
-      </c>
-      <c r="B13" t="s">
-        <v>164</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1762,7 +1762,7 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G13" t="s">
         <v>42</v>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B16" t="s">
         <v>99</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
         <v>120</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
         <v>63</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
         <v>133</v>
@@ -2095,13 +2095,13 @@
         <v>70</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G25" t="s">
         <v>56</v>
       </c>
       <c r="H25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>132</v>
@@ -2145,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2158,7 +2158,7 @@
         <v>70</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G27" t="s">
         <v>56</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B28" t="s">
         <v>84</v>
@@ -2250,7 +2250,7 @@
         <v>26</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>102</v>
@@ -2273,7 +2273,7 @@
         <v>26</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>159</v>
@@ -2388,9 +2388,11 @@
     <hyperlink ref="I8" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="J35" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="I35" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="J11" r:id="rId39" xr:uid="{9DDA845D-E7F0-486E-8EAA-655CA841B46B}"/>
+    <hyperlink ref="I11" r:id="rId40" xr:uid="{7E29F4DF-39D0-4A73-AED1-349F3D032368}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -2398,9 +2400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2539,7 +2539,7 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2580,16 +2580,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" t="s">
         <v>162</v>
       </c>
-      <c r="B9" t="s">
-        <v>164</v>
-      </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
         <v>42</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
         <v>120</v>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
         <v>63</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
         <v>133</v>
@@ -2778,13 +2778,13 @@
         <v>70</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F18" t="s">
         <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2816,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2825,7 +2825,7 @@
         <v>70</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F20" t="s">
         <v>56</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
@@ -2875,7 +2875,7 @@
         <v>26</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I22" s="1"/>
     </row>
@@ -2893,7 +2893,7 @@
         <v>26</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I23" s="1"/>
     </row>
@@ -2937,9 +2937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>